<commit_message>
Graphs for airports and air operators working
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A7109A-2DE8-4606-A49D-FC7EEA783EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58C0DF5-BB36-43E1-8E38-D5426F099D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$254</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$254</definedName>
   </definedNames>
   <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="503">
   <si>
     <t>AG</t>
   </si>
@@ -1742,6 +1742,9 @@
   </si>
   <si>
     <t>EUROCONTROL_REGION</t>
+  </si>
+  <si>
+    <t>CUSTOM</t>
   </si>
 </sst>
 </file>
@@ -2105,12 +2108,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H254"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2123,7 @@
     <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>468</v>
       </c>
@@ -2146,8 +2148,11 @@
       <c r="H1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>252</v>
       </c>
@@ -2173,7 +2178,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -2198,8 +2203,11 @@
       <c r="H3" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2224,8 +2232,11 @@
       <c r="H4" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2251,7 +2262,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>359</v>
       </c>
@@ -2277,7 +2288,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>318</v>
       </c>
@@ -2303,7 +2314,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>398</v>
       </c>
@@ -2328,8 +2339,11 @@
       <c r="H8" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>456</v>
       </c>
@@ -2355,7 +2369,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -2380,8 +2394,11 @@
       <c r="H10" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>394</v>
       </c>
@@ -2406,8 +2423,11 @@
       <c r="H11" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>480</v>
       </c>
@@ -2432,8 +2452,11 @@
       <c r="H12" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>481</v>
       </c>
@@ -2458,8 +2481,11 @@
       <c r="H13" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>482</v>
       </c>
@@ -2484,8 +2510,11 @@
       <c r="H14" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>483</v>
       </c>
@@ -2510,8 +2539,11 @@
       <c r="H15" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>484</v>
       </c>
@@ -2536,8 +2568,11 @@
       <c r="H16" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>485</v>
       </c>
@@ -2562,8 +2597,11 @@
       <c r="H17" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>486</v>
       </c>
@@ -2588,8 +2626,11 @@
       <c r="H18" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>487</v>
       </c>
@@ -2614,8 +2655,11 @@
       <c r="H19" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>488</v>
       </c>
@@ -2640,8 +2684,11 @@
       <c r="H20" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>487</v>
       </c>
@@ -2666,8 +2713,11 @@
       <c r="H21" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>228</v>
       </c>
@@ -2693,7 +2743,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>254</v>
       </c>
@@ -2719,7 +2769,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>416</v>
       </c>
@@ -2745,7 +2795,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>361</v>
       </c>
@@ -2771,7 +2821,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>404</v>
       </c>
@@ -2797,7 +2847,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -2822,8 +2872,11 @@
       <c r="H27" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>230</v>
       </c>
@@ -2849,7 +2902,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -2875,7 +2928,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>430</v>
       </c>
@@ -2901,7 +2954,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>340</v>
       </c>
@@ -2927,7 +2980,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>182</v>
       </c>
@@ -2952,8 +3005,11 @@
       <c r="H32" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>60</v>
       </c>
@@ -2979,7 +3035,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>355</v>
       </c>
@@ -3005,7 +3061,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>349</v>
       </c>
@@ -3031,7 +3087,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>344</v>
       </c>
@@ -3057,7 +3113,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>336</v>
       </c>
@@ -3083,7 +3139,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>334</v>
       </c>
@@ -3109,7 +3165,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>324</v>
       </c>
@@ -3135,7 +3191,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>320</v>
       </c>
@@ -3161,7 +3217,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -3187,7 +3243,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>442</v>
       </c>
@@ -3213,7 +3269,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>156</v>
       </c>
@@ -3238,8 +3294,11 @@
       <c r="H43" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -3265,7 +3324,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>130</v>
       </c>
@@ -3291,7 +3350,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>412</v>
       </c>
@@ -3317,7 +3376,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
@@ -3343,7 +3402,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -3369,7 +3428,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>107</v>
       </c>
@@ -3395,7 +3454,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>126</v>
       </c>
@@ -3421,7 +3480,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>376</v>
       </c>
@@ -3447,7 +3506,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>226</v>
       </c>
@@ -3473,7 +3532,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
@@ -3499,7 +3558,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>91</v>
       </c>
@@ -3525,7 +3584,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>332</v>
       </c>
@@ -3551,7 +3610,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>322</v>
       </c>
@@ -3577,7 +3636,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>338</v>
       </c>
@@ -3603,7 +3662,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>80</v>
       </c>
@@ -3629,7 +3688,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>152</v>
       </c>
@@ -3655,7 +3714,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>232</v>
       </c>
@@ -3681,7 +3740,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>218</v>
       </c>
@@ -3707,7 +3766,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -3733,7 +3792,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>160</v>
       </c>
@@ -3758,8 +3817,11 @@
       <c r="H63" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>224</v>
       </c>
@@ -3785,7 +3847,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>158</v>
       </c>
@@ -3810,8 +3872,11 @@
       <c r="H65" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>171</v>
       </c>
@@ -3836,8 +3901,11 @@
       <c r="H66" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>101</v>
       </c>
@@ -3863,7 +3931,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
@@ -3888,8 +3956,11 @@
       <c r="H68" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
@@ -3915,7 +3986,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>363</v>
       </c>
@@ -3941,7 +4012,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>204</v>
       </c>
@@ -3967,7 +4038,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>326</v>
       </c>
@@ -3993,7 +4064,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>136</v>
       </c>
@@ -4018,8 +4089,11 @@
       <c r="H73" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>220</v>
       </c>
@@ -4045,7 +4119,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>68</v>
       </c>
@@ -4071,7 +4145,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>138</v>
       </c>
@@ -4097,7 +4171,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
@@ -4122,8 +4196,11 @@
       <c r="H77" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>64</v>
       </c>
@@ -4149,7 +4226,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>128</v>
       </c>
@@ -4175,7 +4252,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>304</v>
       </c>
@@ -4201,7 +4278,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>234</v>
       </c>
@@ -4227,7 +4304,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
@@ -4252,8 +4329,11 @@
       <c r="H82" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>163</v>
       </c>
@@ -4278,8 +4358,11 @@
       <c r="H83" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>244</v>
       </c>
@@ -4305,7 +4388,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>248</v>
       </c>
@@ -4331,7 +4414,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>240</v>
       </c>
@@ -4357,7 +4440,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>346</v>
       </c>
@@ -4383,7 +4466,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>83</v>
       </c>
@@ -4409,7 +4492,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>400</v>
       </c>
@@ -4434,8 +4517,11 @@
       <c r="H89" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
@@ -4460,8 +4546,11 @@
       <c r="H90" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>34</v>
       </c>
@@ -4486,8 +4575,11 @@
       <c r="H91" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>20</v>
       </c>
@@ -4513,7 +4605,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>196</v>
       </c>
@@ -4538,8 +4630,11 @@
       <c r="H93" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I93" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>164</v>
       </c>
@@ -4564,8 +4659,11 @@
       <c r="H94" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>6</v>
       </c>
@@ -4591,7 +4689,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>366</v>
       </c>
@@ -4617,7 +4715,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>206</v>
       </c>
@@ -4643,7 +4741,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>124</v>
       </c>
@@ -4669,7 +4767,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>112</v>
       </c>
@@ -4695,7 +4793,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>357</v>
       </c>
@@ -4721,7 +4819,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>222</v>
       </c>
@@ -4747,7 +4845,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>208</v>
       </c>
@@ -4773,7 +4871,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>418</v>
       </c>
@@ -4799,7 +4897,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>166</v>
       </c>
@@ -4824,8 +4922,11 @@
       <c r="H104" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>8</v>
       </c>
@@ -4851,7 +4952,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>414</v>
       </c>
@@ -4877,7 +4978,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>420</v>
       </c>
@@ -4903,7 +5004,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>428</v>
       </c>
@@ -4929,7 +5030,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>408</v>
       </c>
@@ -4955,7 +5056,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>452</v>
       </c>
@@ -4981,7 +5082,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>450</v>
       </c>
@@ -5007,7 +5108,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>444</v>
       </c>
@@ -5033,7 +5134,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>440</v>
       </c>
@@ -5059,7 +5160,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>258</v>
       </c>
@@ -5085,7 +5186,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>272</v>
       </c>
@@ -5111,7 +5212,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
@@ -5136,8 +5237,11 @@
       <c r="H116" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I116" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>173</v>
       </c>
@@ -5162,8 +5266,11 @@
       <c r="H117" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I117" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>168</v>
       </c>
@@ -5188,8 +5295,11 @@
       <c r="H118" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>210</v>
       </c>
@@ -5215,7 +5325,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>310</v>
       </c>
@@ -5241,7 +5351,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>314</v>
       </c>
@@ -5267,7 +5377,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>260</v>
       </c>
@@ -5292,8 +5402,11 @@
       <c r="H122" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>392</v>
       </c>
@@ -5319,7 +5432,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>140</v>
       </c>
@@ -5345,7 +5458,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>284</v>
       </c>
@@ -5371,7 +5484,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>236</v>
       </c>
@@ -5397,7 +5510,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>296</v>
       </c>
@@ -5423,7 +5536,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>10</v>
       </c>
@@ -5449,7 +5562,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>262</v>
       </c>
@@ -5475,7 +5588,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>396</v>
       </c>
@@ -5501,7 +5614,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>422</v>
       </c>
@@ -5527,7 +5640,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>54</v>
       </c>
@@ -5552,8 +5665,11 @@
       <c r="H132" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>264</v>
       </c>
@@ -5578,8 +5694,11 @@
       <c r="H133" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>97</v>
       </c>
@@ -5605,7 +5724,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>114</v>
       </c>
@@ -5631,7 +5750,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>142</v>
       </c>
@@ -5656,8 +5775,11 @@
       <c r="H136" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I136" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>56</v>
       </c>
@@ -5682,8 +5804,11 @@
       <c r="H137" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I137" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>45</v>
       </c>
@@ -5708,8 +5833,11 @@
       <c r="H138" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>424</v>
       </c>
@@ -5735,7 +5863,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>489</v>
       </c>
@@ -5760,8 +5888,11 @@
       <c r="H140" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>491</v>
       </c>
@@ -5786,8 +5917,11 @@
       <c r="H141" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>458</v>
       </c>
@@ -5813,7 +5947,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>95</v>
       </c>
@@ -5839,7 +5973,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>446</v>
       </c>
@@ -5865,7 +5999,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>432</v>
       </c>
@@ -5891,7 +6025,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>103</v>
       </c>
@@ -5917,7 +6051,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>175</v>
       </c>
@@ -5942,8 +6076,11 @@
       <c r="H147" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>294</v>
       </c>
@@ -5969,7 +6106,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>120</v>
       </c>
@@ -5995,7 +6132,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>72</v>
       </c>
@@ -6021,7 +6158,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>473</v>
       </c>
@@ -6047,7 +6184,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>212</v>
       </c>
@@ -6073,7 +6210,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>190</v>
       </c>
@@ -6098,8 +6235,11 @@
       <c r="H153" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I153" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>177</v>
       </c>
@@ -6124,8 +6264,11 @@
       <c r="H154" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>462</v>
       </c>
@@ -6151,7 +6294,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>116</v>
       </c>
@@ -6176,8 +6319,11 @@
       <c r="H156" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>87</v>
       </c>
@@ -6203,7 +6349,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>438</v>
       </c>
@@ -6229,7 +6375,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>99</v>
       </c>
@@ -6255,7 +6401,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>2</v>
       </c>
@@ -6281,7 +6427,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>426</v>
       </c>
@@ -6307,7 +6453,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>40</v>
       </c>
@@ -6332,8 +6478,11 @@
       <c r="H162" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>250</v>
       </c>
@@ -6359,7 +6508,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>214</v>
       </c>
@@ -6385,7 +6534,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>26</v>
       </c>
@@ -6411,7 +6560,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>24</v>
       </c>
@@ -6437,7 +6586,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>238</v>
       </c>
@@ -6463,7 +6612,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>460</v>
       </c>
@@ -6489,7 +6638,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>194</v>
       </c>
@@ -6514,8 +6663,11 @@
       <c r="H169" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I169" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>47</v>
       </c>
@@ -6540,8 +6692,11 @@
       <c r="H170" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>268</v>
       </c>
@@ -6567,7 +6722,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>270</v>
       </c>
@@ -6593,7 +6748,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>192</v>
       </c>
@@ -6618,8 +6773,11 @@
       <c r="H173" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>216</v>
       </c>
@@ -6645,7 +6803,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>4</v>
       </c>
@@ -6671,7 +6829,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>330</v>
       </c>
@@ -6697,7 +6855,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>347</v>
       </c>
@@ -6723,7 +6881,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>316</v>
       </c>
@@ -6749,7 +6907,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>49</v>
       </c>
@@ -6774,8 +6932,11 @@
       <c r="H179" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I179" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>181</v>
       </c>
@@ -6800,8 +6961,11 @@
       <c r="H180" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>276</v>
       </c>
@@ -6827,7 +6991,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>308</v>
       </c>
@@ -6853,7 +7017,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -6879,7 +7043,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>477</v>
       </c>
@@ -6905,7 +7069,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>478</v>
       </c>
@@ -6931,7 +7095,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>184</v>
       </c>
@@ -6956,8 +7120,11 @@
       <c r="H186" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I186" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>390</v>
       </c>
@@ -6983,7 +7150,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>144</v>
       </c>
@@ -7009,7 +7176,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>70</v>
       </c>
@@ -7035,7 +7202,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>372</v>
       </c>
@@ -7061,7 +7228,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>374</v>
       </c>
@@ -7087,7 +7254,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>386</v>
       </c>
@@ -7113,7 +7280,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>242</v>
       </c>
@@ -7139,7 +7306,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>85</v>
       </c>
@@ -7165,7 +7332,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>256</v>
       </c>
@@ -7191,7 +7358,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>118</v>
       </c>
@@ -7217,7 +7384,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>198</v>
       </c>
@@ -7242,8 +7409,11 @@
       <c r="H197" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I197" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>89</v>
       </c>
@@ -7269,7 +7439,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>110</v>
       </c>
@@ -7295,7 +7465,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>454</v>
       </c>
@@ -7321,7 +7491,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>200</v>
       </c>
@@ -7346,8 +7516,11 @@
       <c r="H201" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I201" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>169</v>
       </c>
@@ -7372,8 +7545,11 @@
       <c r="H202" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I202" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>0</v>
       </c>
@@ -7399,7 +7575,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>132</v>
       </c>
@@ -7425,7 +7601,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>58</v>
       </c>
@@ -7451,7 +7627,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>312</v>
       </c>
@@ -7477,7 +7653,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>162</v>
       </c>
@@ -7502,8 +7678,11 @@
       <c r="H207" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I207" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>108</v>
       </c>
@@ -7529,7 +7708,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>410</v>
       </c>
@@ -7555,7 +7734,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>146</v>
       </c>
@@ -7581,7 +7760,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>342</v>
       </c>
@@ -7607,7 +7786,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>51</v>
       </c>
@@ -7632,8 +7811,11 @@
       <c r="H212" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I212" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>186</v>
       </c>
@@ -7658,8 +7840,11 @@
       <c r="H213" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I213" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>274</v>
       </c>
@@ -7684,8 +7869,11 @@
       <c r="H214" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I214" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>406</v>
       </c>
@@ -7711,7 +7899,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>148</v>
       </c>
@@ -7737,7 +7925,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>434</v>
       </c>
@@ -7763,7 +7951,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>105</v>
       </c>
@@ -7789,7 +7977,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>448</v>
       </c>
@@ -7815,7 +8003,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>30</v>
       </c>
@@ -7841,7 +8029,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>382</v>
       </c>
@@ -7867,7 +8055,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>28</v>
       </c>
@@ -7892,8 +8080,11 @@
       <c r="H222" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I222" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>188</v>
       </c>
@@ -7918,8 +8109,11 @@
       <c r="H223" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I223" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>202</v>
       </c>
@@ -7945,7 +8139,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>150</v>
       </c>
@@ -7971,7 +8165,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>378</v>
       </c>
@@ -7997,7 +8191,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>388</v>
       </c>
@@ -8023,7 +8217,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>384</v>
       </c>
@@ -8049,7 +8243,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>380</v>
       </c>
@@ -8075,7 +8269,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>402</v>
       </c>
@@ -8100,8 +8294,11 @@
       <c r="H230" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I230" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>266</v>
       </c>
@@ -8127,7 +8324,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>39</v>
       </c>
@@ -8152,8 +8349,11 @@
       <c r="H232" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I232" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>328</v>
       </c>
@@ -8179,7 +8379,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>351</v>
       </c>
@@ -8205,7 +8405,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>302</v>
       </c>
@@ -8231,7 +8431,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>300</v>
       </c>
@@ -8257,7 +8457,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>286</v>
       </c>
@@ -8283,7 +8483,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>280</v>
       </c>
@@ -8309,7 +8509,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>282</v>
       </c>
@@ -8335,7 +8535,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>288</v>
       </c>
@@ -8735,14 +8935,7 @@
       <c r="G256" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H254" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H254">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I254" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored Departure/Destination region. Able to mix and match regions as well as define additional regions
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0EB00F-1F40-47A3-A198-6985973B8482}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4D9C9-D130-4B50-9E6F-BD3FDA5C2B9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
@@ -2124,7 +2124,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12:G250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,8 +2133,9 @@
     <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2606,7 +2607,7 @@
         <v>463</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>463</v>
@@ -2647,7 +2648,7 @@
         <v>463</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>463</v>
@@ -2688,9 +2689,9 @@
         <v>463</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G14" t="s">
+        <v>455</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>463</v>
       </c>
       <c r="H14" t="s">
@@ -2699,7 +2700,7 @@
       <c r="I14" t="s">
         <v>455</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -2729,7 +2730,7 @@
         <v>463</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>463</v>
@@ -2740,7 +2741,7 @@
       <c r="I15" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -2770,7 +2771,7 @@
         <v>463</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>463</v>
@@ -2811,7 +2812,7 @@
         <v>463</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>463</v>
@@ -2852,7 +2853,7 @@
         <v>463</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>463</v>
@@ -2893,9 +2894,9 @@
         <v>463</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G19" t="s">
+        <v>455</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>463</v>
       </c>
       <c r="H19" t="s">
@@ -2904,7 +2905,7 @@
       <c r="I19" t="s">
         <v>455</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -2934,7 +2935,7 @@
         <v>463</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>463</v>
@@ -2945,7 +2946,7 @@
       <c r="I20" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -2975,7 +2976,7 @@
         <v>463</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>463</v>
@@ -4123,9 +4124,9 @@
         <v>463</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G49" t="s">
+        <v>455</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>463</v>
       </c>
       <c r="H49" t="s">
@@ -4134,7 +4135,7 @@
       <c r="I49" t="s">
         <v>455</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K49" t="s">
@@ -5681,9 +5682,9 @@
         <v>463</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G87" t="s">
+        <v>455</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>463</v>
       </c>
       <c r="H87" t="s">
@@ -5692,7 +5693,7 @@
       <c r="I87" t="s">
         <v>455</v>
       </c>
-      <c r="J87" t="s">
+      <c r="J87" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K87" t="s">
@@ -7854,7 +7855,7 @@
         <v>463</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>463</v>
@@ -7895,7 +7896,7 @@
         <v>463</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>463</v>
@@ -8305,9 +8306,9 @@
         <v>463</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G151" t="s">
+        <v>455</v>
+      </c>
+      <c r="G151" s="2" t="s">
         <v>463</v>
       </c>
       <c r="H151" t="s">
@@ -8316,7 +8317,7 @@
       <c r="I151" t="s">
         <v>455</v>
       </c>
-      <c r="J151" t="s">
+      <c r="J151" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K151" t="s">
@@ -9658,7 +9659,7 @@
         <v>463</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G184" s="2" t="s">
         <v>463</v>
@@ -9669,7 +9670,7 @@
       <c r="I184" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="J184" s="1" t="s">
+      <c r="J184" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K184" s="2" t="s">
@@ -9699,7 +9700,7 @@
         <v>463</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="G185" s="2" t="s">
         <v>463</v>
@@ -12364,9 +12365,9 @@
         <v>463</v>
       </c>
       <c r="F250" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G250" t="s">
+        <v>455</v>
+      </c>
+      <c r="G250" s="2" t="s">
         <v>463</v>
       </c>
       <c r="H250" t="s">
@@ -12375,7 +12376,7 @@
       <c r="I250" t="s">
         <v>455</v>
       </c>
-      <c r="J250" t="s">
+      <c r="J250" s="2" t="s">
         <v>463</v>
       </c>
       <c r="K250" t="s">

</xml_diff>

<commit_message>
Now system averages all flights to and from each Departing region taking into account whether ETD, SAF or ETS applies.
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6752CAD9-E63A-4F9B-93D7-3BBF9DED6CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78D9335-83CD-4922-913D-1AE61CB52F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3735" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2134,7 +2134,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B232" sqref="B232"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12:C250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,7 +2231,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>395</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>391</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>476</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>468</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>453</v>
@@ -2641,7 +2641,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>477</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>468</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>453</v>
@@ -2682,7 +2682,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>478</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>468</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>453</v>
@@ -2723,7 +2723,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>479</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>468</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>453</v>
@@ -2764,7 +2764,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>480</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>468</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>453</v>
@@ -2805,7 +2805,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>481</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>468</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>453</v>
@@ -2846,7 +2846,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>482</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>468</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>453</v>
@@ -2887,7 +2887,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>483</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>468</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>453</v>
@@ -2928,7 +2928,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>484</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>468</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>453</v>
@@ -2969,7 +2969,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>483</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>468</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>453</v>
@@ -3215,7 +3215,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>182</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>156</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>107</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>494</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>453</v>
@@ -4691,7 +4691,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>160</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>158</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>171</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>163</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>343</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>493</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>453</v>
@@ -5757,7 +5757,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>397</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>34</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>196</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>164</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>166</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>8</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>168</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>54</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>56</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>45</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>485</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>486</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>453</v>
@@ -7889,7 +7889,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>487</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>486</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>453</v>
@@ -8135,7 +8135,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>175</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>469</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>470</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>453</v>
@@ -8381,7 +8381,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>190</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>177</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>40</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>194</v>
       </c>
@@ -9078,7 +9078,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>47</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>49</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>181</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>473</v>
       </c>
@@ -9660,7 +9660,7 @@
         <v>472</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>453</v>
@@ -9693,7 +9693,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>474</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>472</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>453</v>
@@ -9734,7 +9734,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>184</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>198</v>
       </c>
@@ -10349,7 +10349,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>199</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>169</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>162</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>51</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>186</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>188</v>
       </c>
@@ -11538,7 +11538,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>399</v>
       </c>
@@ -11620,7 +11620,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>39</v>
       </c>
@@ -12358,7 +12358,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="250" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>362</v>
       </c>
@@ -12366,7 +12366,7 @@
         <v>495</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>453</v>
@@ -12563,7 +12563,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>508</v>
       </c>
@@ -12604,7 +12604,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>509</v>
       </c>
@@ -12647,7 +12647,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M256" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
-    <filterColumn colId="7">
+    <filterColumn colId="8">
       <filters>
         <filter val="Y"/>
       </filters>

</xml_diff>

<commit_message>
various bug fixes in selection filters
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFEC3D5-3165-4EA0-A5EC-37C8FFFEB5D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D2F7F-25EC-4178-8B62-78C4C21A210D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
+    <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2137,7 +2137,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C266" sqref="C266:C267"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,22 +2640,22 @@
         <v>453</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M12" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N12" t="s">
         <v>453</v>
@@ -2684,22 +2684,22 @@
         <v>453</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M13" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N13" t="s">
         <v>453</v>
@@ -2728,22 +2728,22 @@
         <v>453</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I14" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J14" t="s">
         <v>453</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M14" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N14" t="s">
         <v>453</v>
@@ -2772,22 +2772,22 @@
         <v>453</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M15" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N15" t="s">
         <v>453</v>
@@ -2816,22 +2816,22 @@
         <v>453</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M16" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N16" t="s">
         <v>453</v>
@@ -2860,22 +2860,22 @@
         <v>453</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M17" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N17" t="s">
         <v>453</v>
@@ -2904,22 +2904,22 @@
         <v>453</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M18" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N18" t="s">
         <v>453</v>
@@ -2948,22 +2948,22 @@
         <v>453</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I19" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J19" t="s">
         <v>453</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M19" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N19" t="s">
         <v>453</v>
@@ -2992,22 +2992,22 @@
         <v>453</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M20" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N20" t="s">
         <v>453</v>
@@ -3036,22 +3036,22 @@
         <v>453</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M21" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N21" t="s">
         <v>453</v>
@@ -4214,22 +4214,22 @@
         <v>453</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I49" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J49" t="s">
         <v>453</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L49" t="s">
         <v>453</v>
       </c>
       <c r="M49" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N49" t="s">
         <v>453</v>
@@ -5812,22 +5812,22 @@
         <v>453</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I87" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J87" t="s">
         <v>453</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L87" t="s">
         <v>461</v>
       </c>
       <c r="M87" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N87" t="s">
         <v>461</v>
@@ -8040,22 +8040,22 @@
         <v>453</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J140" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K140" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M140" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N140" t="s">
         <v>453</v>
@@ -8084,22 +8084,22 @@
         <v>453</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J141" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K141" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L141" s="2" t="s">
         <v>453</v>
       </c>
       <c r="M141" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N141" t="s">
         <v>453</v>
@@ -8506,22 +8506,22 @@
         <v>453</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I151" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I151" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J151" t="s">
         <v>453</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L151" t="s">
         <v>461</v>
       </c>
       <c r="M151" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N151" t="s">
         <v>461</v>
@@ -9894,22 +9894,22 @@
         <v>453</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I184" s="1" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I184" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J184" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K184" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L184" s="2" t="s">
         <v>461</v>
       </c>
       <c r="M184" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N184" t="s">
         <v>461</v>
@@ -9938,22 +9938,22 @@
         <v>453</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="J185" s="2" t="s">
         <v>453</v>
       </c>
       <c r="K185" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L185" s="2" t="s">
         <v>461</v>
       </c>
       <c r="M185" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N185" t="s">
         <v>461</v>
@@ -12670,22 +12670,22 @@
         <v>453</v>
       </c>
       <c r="H250" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="I250" t="s">
-        <v>461</v>
+        <v>453</v>
+      </c>
+      <c r="I250" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="J250" t="s">
         <v>453</v>
       </c>
       <c r="K250" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="L250" t="s">
         <v>461</v>
       </c>
       <c r="M250" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="N250" t="s">
         <v>461</v>

</xml_diff>

<commit_message>
Added barebones simulation functionality
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D2F7F-25EC-4178-8B62-78C4C21A210D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F7837C-1C98-4268-97DA-8CC799408A22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
@@ -2137,7 +2137,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="E261" sqref="E261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,7 +2617,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>476</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>477</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>478</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>479</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>480</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>481</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>482</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>483</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>484</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>483</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>107</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>343</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>8</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>453</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>453</v>
@@ -8017,7 +8017,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>485</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>487</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>469</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>473</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>474</v>
       </c>
@@ -12647,7 +12647,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>362</v>
       </c>
@@ -12945,9 +12945,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N256" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
-    <filterColumn colId="9">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Y"/>
+        <filter val="Iceland"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Fixed SAF cumulative calculation bug.
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F7837C-1C98-4268-97DA-8CC799408A22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482F3C9-02F3-4CDB-B19E-CA9E613B8483}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
+    <workbookView xWindow="5412" yWindow="5412" windowWidth="28800" windowHeight="15552" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2140,20 +2140,20 @@
       <selection pane="bottomLeft" activeCell="E261" sqref="E261"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>464</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>251</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>356</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>316</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>395</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>453</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>391</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>476</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>477</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>478</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>479</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>480</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>481</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>482</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>483</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>484</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>483</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>227</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>253</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>413</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>358</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>401</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>229</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>427</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>337</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>182</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>60</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>352</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>346</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>341</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>333</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>331</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>321</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>317</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>439</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>156</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>130</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>409</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>107</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>126</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>373</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>225</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>91</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>329</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>319</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>335</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>80</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>152</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>231</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>217</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>160</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>223</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>158</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>171</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>101</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>360</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>203</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>323</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>136</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>219</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>68</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>138</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>64</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>128</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>302</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>233</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>163</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>243</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>247</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>239</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>343</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>83</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>397</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>34</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>20</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>196</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>164</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>6</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>363</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>205</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>124</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>112</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>354</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>221</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>207</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>415</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>166</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>8</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>453</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>453</v>
@@ -6589,7 +6589,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>411</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>417</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>425</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>405</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>449</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>447</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>441</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>437</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>257</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>270</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>173</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>168</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>209</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>308</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>312</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>259</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>389</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>140</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>282</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>235</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>294</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>10</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>260</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>393</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>419</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>54</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>262</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>97</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>114</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>142</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>56</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>45</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>421</v>
       </c>
@@ -8017,7 +8017,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>485</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>487</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>454</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>95</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>443</v>
       </c>
@@ -8231,7 +8231,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>429</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>103</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>175</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>292</v>
       </c>
@@ -8399,7 +8399,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>120</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>72</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>469</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>211</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>190</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>177</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>458</v>
       </c>
@@ -8695,7 +8695,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>116</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>87</v>
       </c>
@@ -8779,7 +8779,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>435</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>99</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>2</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>423</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>40</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>249</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>213</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>26</v>
       </c>
@@ -9115,7 +9115,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>24</v>
       </c>
@@ -9157,7 +9157,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>237</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>456</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>194</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>47</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>266</v>
       </c>
@@ -9367,7 +9367,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>268</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>192</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>215</v>
       </c>
@@ -9493,7 +9493,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>4</v>
       </c>
@@ -9535,7 +9535,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>327</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>344</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>314</v>
       </c>
@@ -9661,7 +9661,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>49</v>
       </c>
@@ -9703,7 +9703,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>181</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>274</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>306</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>473</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>474</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>184</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>387</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>144</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>70</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>369</v>
       </c>
@@ -10169,7 +10169,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>371</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>383</v>
       </c>
@@ -10253,7 +10253,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>241</v>
       </c>
@@ -10295,7 +10295,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>85</v>
       </c>
@@ -10337,7 +10337,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>255</v>
       </c>
@@ -10379,7 +10379,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>118</v>
       </c>
@@ -10421,7 +10421,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>198</v>
       </c>
@@ -10463,7 +10463,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>89</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>110</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>451</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>199</v>
       </c>
@@ -10631,7 +10631,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>169</v>
       </c>
@@ -10673,7 +10673,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>0</v>
       </c>
@@ -10715,7 +10715,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>132</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>58</v>
       </c>
@@ -10799,7 +10799,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>310</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>162</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>108</v>
       </c>
@@ -10925,7 +10925,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>407</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>146</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>339</v>
       </c>
@@ -11051,7 +11051,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>51</v>
       </c>
@@ -11093,7 +11093,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>186</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -11177,7 +11177,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>403</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>148</v>
       </c>
@@ -11261,7 +11261,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>431</v>
       </c>
@@ -11303,7 +11303,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>105</v>
       </c>
@@ -11345,7 +11345,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>445</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>30</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>379</v>
       </c>
@@ -11471,7 +11471,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>28</v>
       </c>
@@ -11513,7 +11513,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>188</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>201</v>
       </c>
@@ -11597,7 +11597,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>150</v>
       </c>
@@ -11639,7 +11639,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>375</v>
       </c>
@@ -11681,7 +11681,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>385</v>
       </c>
@@ -11723,7 +11723,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>381</v>
       </c>
@@ -11765,7 +11765,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>377</v>
       </c>
@@ -11807,7 +11807,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>399</v>
       </c>
@@ -11849,7 +11849,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>264</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>39</v>
       </c>
@@ -11933,7 +11933,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>325</v>
       </c>
@@ -11975,7 +11975,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>348</v>
       </c>
@@ -12017,7 +12017,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>300</v>
       </c>
@@ -12059,7 +12059,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>298</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>284</v>
       </c>
@@ -12143,7 +12143,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>278</v>
       </c>
@@ -12185,7 +12185,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>280</v>
       </c>
@@ -12227,7 +12227,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>286</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>288</v>
       </c>
@@ -12311,7 +12311,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>290</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>296</v>
       </c>
@@ -12395,7 +12395,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>367</v>
       </c>
@@ -12437,7 +12437,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>365</v>
       </c>
@@ -12479,7 +12479,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>304</v>
       </c>
@@ -12521,7 +12521,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>245</v>
       </c>
@@ -12563,7 +12563,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>350</v>
       </c>
@@ -12605,7 +12605,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>433</v>
       </c>
@@ -12647,7 +12647,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>362</v>
       </c>
@@ -12691,7 +12691,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>122</v>
       </c>
@@ -12733,7 +12733,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>276</v>
       </c>
@@ -12775,7 +12775,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>78</v>
       </c>
@@ -12817,7 +12817,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>93</v>
       </c>
@@ -12859,7 +12859,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>508</v>
       </c>
@@ -12901,7 +12901,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>509</v>
       </c>
@@ -12948,6 +12948,8 @@
     <filterColumn colId="2">
       <filters>
         <filter val="Iceland"/>
+        <filter val="Norway"/>
+        <filter val="Switzerland"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Removed Business flight exemption from ETD. Will likely be taxed with whatever rate applies for commercial flights. Added ability to calculate ETS for all departing flights
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482F3C9-02F3-4CDB-B19E-CA9E613B8483}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3634F48-A31F-429B-AE51-F6DA05097734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5412" yWindow="5412" windowWidth="28800" windowHeight="15552" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$256</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$256</definedName>
   </definedNames>
   <calcPr calcId="181029" calcMode="manual"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3347" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="513">
   <si>
     <t>AG</t>
   </si>
@@ -1769,6 +1769,12 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>EEA</t>
   </si>
 </sst>
 </file>
@@ -2133,11 +2139,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N256"/>
+  <dimension ref="A1:P256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E261" sqref="E261"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12:O250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,7 +2159,7 @@
     <col min="13" max="13" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>464</v>
       </c>
@@ -2196,8 +2202,14 @@
       <c r="N1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>511</v>
+      </c>
+      <c r="P1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>251</v>
       </c>
@@ -2238,8 +2250,14 @@
       <c r="N2" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>461</v>
+      </c>
+      <c r="P2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -2280,8 +2298,14 @@
       <c r="N3" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>461</v>
+      </c>
+      <c r="P3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2322,8 +2346,14 @@
       <c r="N4" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>461</v>
+      </c>
+      <c r="P4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2364,8 +2394,14 @@
       <c r="N5" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>461</v>
+      </c>
+      <c r="P5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>356</v>
       </c>
@@ -2406,8 +2442,14 @@
       <c r="N6" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>461</v>
+      </c>
+      <c r="P6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>316</v>
       </c>
@@ -2448,8 +2490,14 @@
       <c r="N7" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>461</v>
+      </c>
+      <c r="P7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>395</v>
       </c>
@@ -2490,8 +2538,14 @@
       <c r="N8" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>461</v>
+      </c>
+      <c r="P8" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>453</v>
       </c>
@@ -2532,8 +2586,14 @@
       <c r="N9" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>461</v>
+      </c>
+      <c r="P9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -2574,8 +2634,14 @@
       <c r="N10" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>453</v>
+      </c>
+      <c r="P10" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>391</v>
       </c>
@@ -2616,8 +2682,14 @@
       <c r="N11" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>461</v>
+      </c>
+      <c r="P11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>476</v>
       </c>
@@ -2660,8 +2732,14 @@
       <c r="N12" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>461</v>
+      </c>
+      <c r="P12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>477</v>
       </c>
@@ -2704,8 +2782,14 @@
       <c r="N13" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>461</v>
+      </c>
+      <c r="P13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>478</v>
       </c>
@@ -2748,8 +2832,14 @@
       <c r="N14" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>461</v>
+      </c>
+      <c r="P14" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>479</v>
       </c>
@@ -2792,8 +2882,14 @@
       <c r="N15" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O15" t="s">
+        <v>461</v>
+      </c>
+      <c r="P15" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>480</v>
       </c>
@@ -2836,8 +2932,14 @@
       <c r="N16" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O16" t="s">
+        <v>461</v>
+      </c>
+      <c r="P16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>481</v>
       </c>
@@ -2880,8 +2982,14 @@
       <c r="N17" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>461</v>
+      </c>
+      <c r="P17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>482</v>
       </c>
@@ -2924,8 +3032,14 @@
       <c r="N18" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>461</v>
+      </c>
+      <c r="P18" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>483</v>
       </c>
@@ -2968,8 +3082,14 @@
       <c r="N19" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>461</v>
+      </c>
+      <c r="P19" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>484</v>
       </c>
@@ -3012,8 +3132,14 @@
       <c r="N20" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>461</v>
+      </c>
+      <c r="P20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>483</v>
       </c>
@@ -3056,8 +3182,14 @@
       <c r="N21" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>461</v>
+      </c>
+      <c r="P21" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>227</v>
       </c>
@@ -3098,8 +3230,14 @@
       <c r="N22" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>461</v>
+      </c>
+      <c r="P22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>253</v>
       </c>
@@ -3140,8 +3278,14 @@
       <c r="N23" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>461</v>
+      </c>
+      <c r="P23" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>413</v>
       </c>
@@ -3182,8 +3326,14 @@
       <c r="N24" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O24" t="s">
+        <v>461</v>
+      </c>
+      <c r="P24" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>358</v>
       </c>
@@ -3224,8 +3374,14 @@
       <c r="N25" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O25" t="s">
+        <v>461</v>
+      </c>
+      <c r="P25" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>401</v>
       </c>
@@ -3266,8 +3422,14 @@
       <c r="N26" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>461</v>
+      </c>
+      <c r="P26" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -3308,8 +3470,14 @@
       <c r="N27" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O27" t="s">
+        <v>453</v>
+      </c>
+      <c r="P27" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>229</v>
       </c>
@@ -3350,8 +3518,14 @@
       <c r="N28" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O28" t="s">
+        <v>461</v>
+      </c>
+      <c r="P28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -3392,8 +3566,14 @@
       <c r="N29" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O29" t="s">
+        <v>461</v>
+      </c>
+      <c r="P29" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>427</v>
       </c>
@@ -3434,8 +3614,14 @@
       <c r="N30" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>461</v>
+      </c>
+      <c r="P30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>337</v>
       </c>
@@ -3476,8 +3662,14 @@
       <c r="N31" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>461</v>
+      </c>
+      <c r="P31" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>182</v>
       </c>
@@ -3518,8 +3710,14 @@
       <c r="N32" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>461</v>
+      </c>
+      <c r="P32" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>60</v>
       </c>
@@ -3560,8 +3758,14 @@
       <c r="N33" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>461</v>
+      </c>
+      <c r="P33" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>352</v>
       </c>
@@ -3602,8 +3806,14 @@
       <c r="N34" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>461</v>
+      </c>
+      <c r="P34" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>346</v>
       </c>
@@ -3644,8 +3854,14 @@
       <c r="N35" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O35" t="s">
+        <v>461</v>
+      </c>
+      <c r="P35" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>341</v>
       </c>
@@ -3686,8 +3902,14 @@
       <c r="N36" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O36" t="s">
+        <v>461</v>
+      </c>
+      <c r="P36" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>333</v>
       </c>
@@ -3728,8 +3950,14 @@
       <c r="N37" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O37" t="s">
+        <v>461</v>
+      </c>
+      <c r="P37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>331</v>
       </c>
@@ -3770,8 +3998,14 @@
       <c r="N38" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O38" t="s">
+        <v>461</v>
+      </c>
+      <c r="P38" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>321</v>
       </c>
@@ -3812,8 +4046,14 @@
       <c r="N39" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O39" t="s">
+        <v>461</v>
+      </c>
+      <c r="P39" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>317</v>
       </c>
@@ -3854,8 +4094,14 @@
       <c r="N40" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O40" t="s">
+        <v>461</v>
+      </c>
+      <c r="P40" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -3896,8 +4142,14 @@
       <c r="N41" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O41" t="s">
+        <v>461</v>
+      </c>
+      <c r="P41" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>439</v>
       </c>
@@ -3938,8 +4190,14 @@
       <c r="N42" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O42" t="s">
+        <v>461</v>
+      </c>
+      <c r="P42" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>156</v>
       </c>
@@ -3980,8 +4238,14 @@
       <c r="N43" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O43" t="s">
+        <v>453</v>
+      </c>
+      <c r="P43" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -4022,8 +4286,14 @@
       <c r="N44" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O44" t="s">
+        <v>461</v>
+      </c>
+      <c r="P44" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>130</v>
       </c>
@@ -4064,8 +4334,14 @@
       <c r="N45" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O45" t="s">
+        <v>461</v>
+      </c>
+      <c r="P45" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>409</v>
       </c>
@@ -4106,8 +4382,14 @@
       <c r="N46" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O46" t="s">
+        <v>461</v>
+      </c>
+      <c r="P46" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
@@ -4148,8 +4430,14 @@
       <c r="N47" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O47" t="s">
+        <v>461</v>
+      </c>
+      <c r="P47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -4190,8 +4478,14 @@
       <c r="N48" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O48" t="s">
+        <v>461</v>
+      </c>
+      <c r="P48" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>107</v>
       </c>
@@ -4234,8 +4528,14 @@
       <c r="N49" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O49" t="s">
+        <v>461</v>
+      </c>
+      <c r="P49" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>126</v>
       </c>
@@ -4276,8 +4576,14 @@
       <c r="N50" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>461</v>
+      </c>
+      <c r="P50" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>373</v>
       </c>
@@ -4318,8 +4624,14 @@
       <c r="N51" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O51" t="s">
+        <v>461</v>
+      </c>
+      <c r="P51" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>225</v>
       </c>
@@ -4360,8 +4672,14 @@
       <c r="N52" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O52" t="s">
+        <v>461</v>
+      </c>
+      <c r="P52" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
@@ -4402,8 +4720,14 @@
       <c r="N53" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O53" t="s">
+        <v>461</v>
+      </c>
+      <c r="P53" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>91</v>
       </c>
@@ -4444,8 +4768,14 @@
       <c r="N54" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O54" t="s">
+        <v>461</v>
+      </c>
+      <c r="P54" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>329</v>
       </c>
@@ -4486,8 +4816,14 @@
       <c r="N55" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O55" t="s">
+        <v>461</v>
+      </c>
+      <c r="P55" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>319</v>
       </c>
@@ -4528,8 +4864,14 @@
       <c r="N56" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O56" t="s">
+        <v>461</v>
+      </c>
+      <c r="P56" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>335</v>
       </c>
@@ -4570,8 +4912,14 @@
       <c r="N57" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O57" t="s">
+        <v>461</v>
+      </c>
+      <c r="P57" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>80</v>
       </c>
@@ -4612,8 +4960,14 @@
       <c r="N58" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O58" t="s">
+        <v>461</v>
+      </c>
+      <c r="P58" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>152</v>
       </c>
@@ -4654,8 +5008,14 @@
       <c r="N59" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O59" t="s">
+        <v>461</v>
+      </c>
+      <c r="P59" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>231</v>
       </c>
@@ -4696,8 +5056,14 @@
       <c r="N60" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O60" t="s">
+        <v>461</v>
+      </c>
+      <c r="P60" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>217</v>
       </c>
@@ -4738,8 +5104,14 @@
       <c r="N61" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O61" t="s">
+        <v>461</v>
+      </c>
+      <c r="P61" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -4780,8 +5152,14 @@
       <c r="N62" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O62" t="s">
+        <v>461</v>
+      </c>
+      <c r="P62" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>160</v>
       </c>
@@ -4822,8 +5200,14 @@
       <c r="N63" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O63" t="s">
+        <v>453</v>
+      </c>
+      <c r="P63" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>223</v>
       </c>
@@ -4864,8 +5248,14 @@
       <c r="N64" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O64" t="s">
+        <v>461</v>
+      </c>
+      <c r="P64" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>158</v>
       </c>
@@ -4906,8 +5296,14 @@
       <c r="N65" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O65" t="s">
+        <v>453</v>
+      </c>
+      <c r="P65" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>171</v>
       </c>
@@ -4948,8 +5344,14 @@
       <c r="N66" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O66" t="s">
+        <v>453</v>
+      </c>
+      <c r="P66" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>101</v>
       </c>
@@ -4990,8 +5392,14 @@
       <c r="N67" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O67" t="s">
+        <v>461</v>
+      </c>
+      <c r="P67" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
@@ -5032,8 +5440,14 @@
       <c r="N68" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O68" t="s">
+        <v>453</v>
+      </c>
+      <c r="P68" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
@@ -5074,8 +5488,14 @@
       <c r="N69" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O69" t="s">
+        <v>461</v>
+      </c>
+      <c r="P69" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>360</v>
       </c>
@@ -5116,8 +5536,14 @@
       <c r="N70" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O70" t="s">
+        <v>461</v>
+      </c>
+      <c r="P70" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>203</v>
       </c>
@@ -5158,8 +5584,14 @@
       <c r="N71" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O71" t="s">
+        <v>461</v>
+      </c>
+      <c r="P71" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>323</v>
       </c>
@@ -5200,8 +5632,14 @@
       <c r="N72" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O72" t="s">
+        <v>461</v>
+      </c>
+      <c r="P72" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>136</v>
       </c>
@@ -5242,8 +5680,14 @@
       <c r="N73" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O73" t="s">
+        <v>461</v>
+      </c>
+      <c r="P73" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>219</v>
       </c>
@@ -5284,8 +5728,14 @@
       <c r="N74" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O74" t="s">
+        <v>461</v>
+      </c>
+      <c r="P74" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>68</v>
       </c>
@@ -5326,8 +5776,14 @@
       <c r="N75" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O75" t="s">
+        <v>461</v>
+      </c>
+      <c r="P75" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>138</v>
       </c>
@@ -5368,8 +5824,14 @@
       <c r="N76" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O76" t="s">
+        <v>461</v>
+      </c>
+      <c r="P76" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
@@ -5410,8 +5872,14 @@
       <c r="N77" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O77" t="s">
+        <v>453</v>
+      </c>
+      <c r="P77" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>64</v>
       </c>
@@ -5452,8 +5920,14 @@
       <c r="N78" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O78" t="s">
+        <v>461</v>
+      </c>
+      <c r="P78" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>128</v>
       </c>
@@ -5494,8 +5968,14 @@
       <c r="N79" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O79" t="s">
+        <v>461</v>
+      </c>
+      <c r="P79" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>302</v>
       </c>
@@ -5536,8 +6016,14 @@
       <c r="N80" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O80" t="s">
+        <v>461</v>
+      </c>
+      <c r="P80" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>233</v>
       </c>
@@ -5578,8 +6064,14 @@
       <c r="N81" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O81" t="s">
+        <v>461</v>
+      </c>
+      <c r="P81" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
@@ -5620,8 +6112,14 @@
       <c r="N82" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O82" t="s">
+        <v>453</v>
+      </c>
+      <c r="P82" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>163</v>
       </c>
@@ -5662,8 +6160,14 @@
       <c r="N83" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O83" t="s">
+        <v>453</v>
+      </c>
+      <c r="P83" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>243</v>
       </c>
@@ -5704,8 +6208,14 @@
       <c r="N84" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O84" t="s">
+        <v>461</v>
+      </c>
+      <c r="P84" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>247</v>
       </c>
@@ -5746,8 +6256,14 @@
       <c r="N85" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O85" t="s">
+        <v>461</v>
+      </c>
+      <c r="P85" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>239</v>
       </c>
@@ -5788,8 +6304,14 @@
       <c r="N86" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O86" t="s">
+        <v>461</v>
+      </c>
+      <c r="P86" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>343</v>
       </c>
@@ -5832,8 +6354,14 @@
       <c r="N87" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O87" t="s">
+        <v>461</v>
+      </c>
+      <c r="P87" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>83</v>
       </c>
@@ -5874,8 +6402,14 @@
       <c r="N88" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O88" t="s">
+        <v>461</v>
+      </c>
+      <c r="P88" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>397</v>
       </c>
@@ -5916,8 +6450,14 @@
       <c r="N89" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O89" t="s">
+        <v>461</v>
+      </c>
+      <c r="P89" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
@@ -5958,8 +6498,14 @@
       <c r="N90" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O90" t="s">
+        <v>453</v>
+      </c>
+      <c r="P90" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>34</v>
       </c>
@@ -6000,8 +6546,14 @@
       <c r="N91" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O91" t="s">
+        <v>453</v>
+      </c>
+      <c r="P91" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>20</v>
       </c>
@@ -6042,8 +6594,14 @@
       <c r="N92" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O92" t="s">
+        <v>461</v>
+      </c>
+      <c r="P92" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>196</v>
       </c>
@@ -6084,8 +6642,14 @@
       <c r="N93" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O93" t="s">
+        <v>461</v>
+      </c>
+      <c r="P93" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>164</v>
       </c>
@@ -6126,8 +6690,14 @@
       <c r="N94" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O94" t="s">
+        <v>453</v>
+      </c>
+      <c r="P94" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>6</v>
       </c>
@@ -6168,8 +6738,14 @@
       <c r="N95" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O95" t="s">
+        <v>461</v>
+      </c>
+      <c r="P95" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>363</v>
       </c>
@@ -6210,8 +6786,14 @@
       <c r="N96" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O96" t="s">
+        <v>461</v>
+      </c>
+      <c r="P96" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>205</v>
       </c>
@@ -6252,8 +6834,14 @@
       <c r="N97" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O97" t="s">
+        <v>461</v>
+      </c>
+      <c r="P97" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>124</v>
       </c>
@@ -6294,8 +6882,14 @@
       <c r="N98" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O98" t="s">
+        <v>461</v>
+      </c>
+      <c r="P98" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>112</v>
       </c>
@@ -6336,8 +6930,14 @@
       <c r="N99" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O99" t="s">
+        <v>461</v>
+      </c>
+      <c r="P99" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>354</v>
       </c>
@@ -6378,8 +6978,14 @@
       <c r="N100" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O100" t="s">
+        <v>461</v>
+      </c>
+      <c r="P100" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>221</v>
       </c>
@@ -6420,8 +7026,14 @@
       <c r="N101" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O101" t="s">
+        <v>461</v>
+      </c>
+      <c r="P101" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>207</v>
       </c>
@@ -6462,8 +7074,14 @@
       <c r="N102" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O102" t="s">
+        <v>461</v>
+      </c>
+      <c r="P102" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>415</v>
       </c>
@@ -6504,8 +7122,14 @@
       <c r="N103" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O103" t="s">
+        <v>461</v>
+      </c>
+      <c r="P103" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>166</v>
       </c>
@@ -6546,8 +7170,14 @@
       <c r="N104" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O104" t="s">
+        <v>453</v>
+      </c>
+      <c r="P104" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>8</v>
       </c>
@@ -6588,8 +7218,14 @@
       <c r="N105" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O105" t="s">
+        <v>461</v>
+      </c>
+      <c r="P105" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>411</v>
       </c>
@@ -6630,8 +7266,14 @@
       <c r="N106" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O106" t="s">
+        <v>461</v>
+      </c>
+      <c r="P106" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>417</v>
       </c>
@@ -6672,8 +7314,14 @@
       <c r="N107" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O107" t="s">
+        <v>461</v>
+      </c>
+      <c r="P107" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>425</v>
       </c>
@@ -6714,8 +7362,14 @@
       <c r="N108" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O108" t="s">
+        <v>461</v>
+      </c>
+      <c r="P108" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>405</v>
       </c>
@@ -6756,8 +7410,14 @@
       <c r="N109" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O109" t="s">
+        <v>461</v>
+      </c>
+      <c r="P109" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>449</v>
       </c>
@@ -6798,8 +7458,14 @@
       <c r="N110" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O110" t="s">
+        <v>461</v>
+      </c>
+      <c r="P110" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>447</v>
       </c>
@@ -6840,8 +7506,14 @@
       <c r="N111" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O111" t="s">
+        <v>461</v>
+      </c>
+      <c r="P111" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>441</v>
       </c>
@@ -6882,8 +7554,14 @@
       <c r="N112" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O112" t="s">
+        <v>461</v>
+      </c>
+      <c r="P112" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>437</v>
       </c>
@@ -6924,8 +7602,14 @@
       <c r="N113" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O113" t="s">
+        <v>461</v>
+      </c>
+      <c r="P113" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>257</v>
       </c>
@@ -6966,8 +7650,14 @@
       <c r="N114" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O114" t="s">
+        <v>461</v>
+      </c>
+      <c r="P114" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>270</v>
       </c>
@@ -7008,8 +7698,14 @@
       <c r="N115" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O115" t="s">
+        <v>461</v>
+      </c>
+      <c r="P115" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
@@ -7050,8 +7746,14 @@
       <c r="N116" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O116" t="s">
+        <v>453</v>
+      </c>
+      <c r="P116" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>173</v>
       </c>
@@ -7092,8 +7794,14 @@
       <c r="N117" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O117" t="s">
+        <v>461</v>
+      </c>
+      <c r="P117" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>168</v>
       </c>
@@ -7134,8 +7842,14 @@
       <c r="N118" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O118" t="s">
+        <v>453</v>
+      </c>
+      <c r="P118" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>209</v>
       </c>
@@ -7176,8 +7890,14 @@
       <c r="N119" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O119" t="s">
+        <v>461</v>
+      </c>
+      <c r="P119" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>308</v>
       </c>
@@ -7218,8 +7938,14 @@
       <c r="N120" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O120" t="s">
+        <v>461</v>
+      </c>
+      <c r="P120" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>312</v>
       </c>
@@ -7260,8 +7986,14 @@
       <c r="N121" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O121" t="s">
+        <v>461</v>
+      </c>
+      <c r="P121" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>259</v>
       </c>
@@ -7302,8 +8034,14 @@
       <c r="N122" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O122" t="s">
+        <v>461</v>
+      </c>
+      <c r="P122" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>389</v>
       </c>
@@ -7344,8 +8082,14 @@
       <c r="N123" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O123" t="s">
+        <v>461</v>
+      </c>
+      <c r="P123" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>140</v>
       </c>
@@ -7386,8 +8130,14 @@
       <c r="N124" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O124" t="s">
+        <v>461</v>
+      </c>
+      <c r="P124" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>282</v>
       </c>
@@ -7428,8 +8178,14 @@
       <c r="N125" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O125" t="s">
+        <v>461</v>
+      </c>
+      <c r="P125" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>235</v>
       </c>
@@ -7470,8 +8226,14 @@
       <c r="N126" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O126" t="s">
+        <v>461</v>
+      </c>
+      <c r="P126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>294</v>
       </c>
@@ -7512,8 +8274,14 @@
       <c r="N127" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O127" t="s">
+        <v>461</v>
+      </c>
+      <c r="P127" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>10</v>
       </c>
@@ -7554,8 +8322,14 @@
       <c r="N128" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O128" t="s">
+        <v>461</v>
+      </c>
+      <c r="P128" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>260</v>
       </c>
@@ -7596,8 +8370,14 @@
       <c r="N129" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O129" t="s">
+        <v>461</v>
+      </c>
+      <c r="P129" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>393</v>
       </c>
@@ -7638,8 +8418,14 @@
       <c r="N130" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O130" t="s">
+        <v>461</v>
+      </c>
+      <c r="P130" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>419</v>
       </c>
@@ -7680,8 +8466,14 @@
       <c r="N131" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O131" t="s">
+        <v>461</v>
+      </c>
+      <c r="P131" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>54</v>
       </c>
@@ -7722,8 +8514,14 @@
       <c r="N132" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O132" t="s">
+        <v>453</v>
+      </c>
+      <c r="P132" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>262</v>
       </c>
@@ -7764,8 +8562,14 @@
       <c r="N133" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O133" t="s">
+        <v>461</v>
+      </c>
+      <c r="P133" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>97</v>
       </c>
@@ -7806,8 +8610,14 @@
       <c r="N134" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O134" t="s">
+        <v>461</v>
+      </c>
+      <c r="P134" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>114</v>
       </c>
@@ -7848,8 +8658,14 @@
       <c r="N135" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O135" t="s">
+        <v>461</v>
+      </c>
+      <c r="P135" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>142</v>
       </c>
@@ -7890,8 +8706,14 @@
       <c r="N136" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O136" t="s">
+        <v>461</v>
+      </c>
+      <c r="P136" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>56</v>
       </c>
@@ -7932,8 +8754,14 @@
       <c r="N137" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O137" t="s">
+        <v>453</v>
+      </c>
+      <c r="P137" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>45</v>
       </c>
@@ -7974,8 +8802,14 @@
       <c r="N138" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O138" t="s">
+        <v>453</v>
+      </c>
+      <c r="P138" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>421</v>
       </c>
@@ -8016,8 +8850,14 @@
       <c r="N139" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O139" t="s">
+        <v>461</v>
+      </c>
+      <c r="P139" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>485</v>
       </c>
@@ -8060,8 +8900,14 @@
       <c r="N140" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O140" t="s">
+        <v>461</v>
+      </c>
+      <c r="P140" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>487</v>
       </c>
@@ -8104,8 +8950,14 @@
       <c r="N141" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O141" t="s">
+        <v>461</v>
+      </c>
+      <c r="P141" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>454</v>
       </c>
@@ -8146,8 +8998,14 @@
       <c r="N142" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O142" t="s">
+        <v>461</v>
+      </c>
+      <c r="P142" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>95</v>
       </c>
@@ -8188,8 +9046,14 @@
       <c r="N143" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O143" t="s">
+        <v>461</v>
+      </c>
+      <c r="P143" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>443</v>
       </c>
@@ -8230,8 +9094,14 @@
       <c r="N144" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O144" t="s">
+        <v>461</v>
+      </c>
+      <c r="P144" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>429</v>
       </c>
@@ -8272,8 +9142,14 @@
       <c r="N145" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O145" t="s">
+        <v>461</v>
+      </c>
+      <c r="P145" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>103</v>
       </c>
@@ -8314,8 +9190,14 @@
       <c r="N146" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O146" t="s">
+        <v>461</v>
+      </c>
+      <c r="P146" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>175</v>
       </c>
@@ -8356,8 +9238,14 @@
       <c r="N147" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O147" t="s">
+        <v>453</v>
+      </c>
+      <c r="P147" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>292</v>
       </c>
@@ -8398,8 +9286,14 @@
       <c r="N148" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O148" t="s">
+        <v>461</v>
+      </c>
+      <c r="P148" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>120</v>
       </c>
@@ -8440,8 +9334,14 @@
       <c r="N149" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O149" t="s">
+        <v>461</v>
+      </c>
+      <c r="P149" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>72</v>
       </c>
@@ -8482,8 +9382,14 @@
       <c r="N150" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O150" t="s">
+        <v>461</v>
+      </c>
+      <c r="P150" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>469</v>
       </c>
@@ -8526,8 +9432,14 @@
       <c r="N151" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O151" t="s">
+        <v>461</v>
+      </c>
+      <c r="P151" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>211</v>
       </c>
@@ -8568,8 +9480,14 @@
       <c r="N152" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O152" t="s">
+        <v>461</v>
+      </c>
+      <c r="P152" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>190</v>
       </c>
@@ -8610,8 +9528,14 @@
       <c r="N153" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O153" t="s">
+        <v>461</v>
+      </c>
+      <c r="P153" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>177</v>
       </c>
@@ -8652,8 +9576,14 @@
       <c r="N154" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O154" t="s">
+        <v>461</v>
+      </c>
+      <c r="P154" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>458</v>
       </c>
@@ -8694,8 +9624,14 @@
       <c r="N155" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O155" t="s">
+        <v>461</v>
+      </c>
+      <c r="P155" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>116</v>
       </c>
@@ -8736,8 +9672,14 @@
       <c r="N156" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O156" t="s">
+        <v>461</v>
+      </c>
+      <c r="P156" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>87</v>
       </c>
@@ -8778,8 +9720,14 @@
       <c r="N157" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O157" t="s">
+        <v>461</v>
+      </c>
+      <c r="P157" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>435</v>
       </c>
@@ -8820,8 +9768,14 @@
       <c r="N158" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O158" t="s">
+        <v>461</v>
+      </c>
+      <c r="P158" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>99</v>
       </c>
@@ -8862,8 +9816,14 @@
       <c r="N159" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O159" t="s">
+        <v>461</v>
+      </c>
+      <c r="P159" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>2</v>
       </c>
@@ -8904,8 +9864,14 @@
       <c r="N160" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O160" t="s">
+        <v>461</v>
+      </c>
+      <c r="P160" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>423</v>
       </c>
@@ -8946,8 +9912,14 @@
       <c r="N161" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O161" t="s">
+        <v>461</v>
+      </c>
+      <c r="P161" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>40</v>
       </c>
@@ -8988,8 +9960,14 @@
       <c r="N162" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O162" t="s">
+        <v>453</v>
+      </c>
+      <c r="P162" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>249</v>
       </c>
@@ -9030,8 +10008,14 @@
       <c r="N163" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O163" t="s">
+        <v>461</v>
+      </c>
+      <c r="P163" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>213</v>
       </c>
@@ -9072,8 +10056,14 @@
       <c r="N164" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O164" t="s">
+        <v>461</v>
+      </c>
+      <c r="P164" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>26</v>
       </c>
@@ -9114,8 +10104,14 @@
       <c r="N165" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O165" t="s">
+        <v>461</v>
+      </c>
+      <c r="P165" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>24</v>
       </c>
@@ -9156,8 +10152,14 @@
       <c r="N166" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O166" t="s">
+        <v>461</v>
+      </c>
+      <c r="P166" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>237</v>
       </c>
@@ -9198,8 +10200,14 @@
       <c r="N167" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O167" t="s">
+        <v>461</v>
+      </c>
+      <c r="P167" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>456</v>
       </c>
@@ -9240,8 +10248,14 @@
       <c r="N168" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O168" t="s">
+        <v>461</v>
+      </c>
+      <c r="P168" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>194</v>
       </c>
@@ -9282,8 +10296,14 @@
       <c r="N169" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O169" t="s">
+        <v>461</v>
+      </c>
+      <c r="P169" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>47</v>
       </c>
@@ -9324,8 +10344,14 @@
       <c r="N170" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O170" t="s">
+        <v>461</v>
+      </c>
+      <c r="P170" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>266</v>
       </c>
@@ -9366,8 +10392,14 @@
       <c r="N171" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O171" t="s">
+        <v>461</v>
+      </c>
+      <c r="P171" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>268</v>
       </c>
@@ -9408,8 +10440,14 @@
       <c r="N172" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O172" t="s">
+        <v>461</v>
+      </c>
+      <c r="P172" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>192</v>
       </c>
@@ -9450,8 +10488,14 @@
       <c r="N173" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O173" t="s">
+        <v>461</v>
+      </c>
+      <c r="P173" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>215</v>
       </c>
@@ -9492,8 +10536,14 @@
       <c r="N174" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O174" t="s">
+        <v>461</v>
+      </c>
+      <c r="P174" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>4</v>
       </c>
@@ -9534,8 +10584,14 @@
       <c r="N175" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O175" t="s">
+        <v>461</v>
+      </c>
+      <c r="P175" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>327</v>
       </c>
@@ -9576,8 +10632,14 @@
       <c r="N176" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O176" t="s">
+        <v>461</v>
+      </c>
+      <c r="P176" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>344</v>
       </c>
@@ -9618,8 +10680,14 @@
       <c r="N177" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O177" t="s">
+        <v>461</v>
+      </c>
+      <c r="P177" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>314</v>
       </c>
@@ -9660,8 +10728,14 @@
       <c r="N178" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O178" t="s">
+        <v>461</v>
+      </c>
+      <c r="P178" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>49</v>
       </c>
@@ -9702,8 +10776,14 @@
       <c r="N179" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O179" t="s">
+        <v>453</v>
+      </c>
+      <c r="P179" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>181</v>
       </c>
@@ -9744,8 +10824,14 @@
       <c r="N180" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O180" t="s">
+        <v>453</v>
+      </c>
+      <c r="P180" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>274</v>
       </c>
@@ -9786,8 +10872,14 @@
       <c r="N181" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O181" t="s">
+        <v>461</v>
+      </c>
+      <c r="P181" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>306</v>
       </c>
@@ -9828,8 +10920,14 @@
       <c r="N182" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O182" t="s">
+        <v>461</v>
+      </c>
+      <c r="P182" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>62</v>
       </c>
@@ -9870,8 +10968,14 @@
       <c r="N183" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O183" t="s">
+        <v>461</v>
+      </c>
+      <c r="P183" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>473</v>
       </c>
@@ -9914,8 +11018,14 @@
       <c r="N184" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O184" t="s">
+        <v>461</v>
+      </c>
+      <c r="P184" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>474</v>
       </c>
@@ -9958,8 +11068,14 @@
       <c r="N185" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O185" t="s">
+        <v>461</v>
+      </c>
+      <c r="P185" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>184</v>
       </c>
@@ -10000,8 +11116,14 @@
       <c r="N186" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="187" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O186" t="s">
+        <v>453</v>
+      </c>
+      <c r="P186" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>387</v>
       </c>
@@ -10042,8 +11164,14 @@
       <c r="N187" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O187" t="s">
+        <v>461</v>
+      </c>
+      <c r="P187" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>144</v>
       </c>
@@ -10084,8 +11212,14 @@
       <c r="N188" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O188" t="s">
+        <v>461</v>
+      </c>
+      <c r="P188" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>70</v>
       </c>
@@ -10126,8 +11260,14 @@
       <c r="N189" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O189" t="s">
+        <v>461</v>
+      </c>
+      <c r="P189" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>369</v>
       </c>
@@ -10168,8 +11308,14 @@
       <c r="N190" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O190" t="s">
+        <v>461</v>
+      </c>
+      <c r="P190" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>371</v>
       </c>
@@ -10210,8 +11356,14 @@
       <c r="N191" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O191" t="s">
+        <v>461</v>
+      </c>
+      <c r="P191" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>383</v>
       </c>
@@ -10252,8 +11404,14 @@
       <c r="N192" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O192" t="s">
+        <v>461</v>
+      </c>
+      <c r="P192" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>241</v>
       </c>
@@ -10294,8 +11452,14 @@
       <c r="N193" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O193" t="s">
+        <v>461</v>
+      </c>
+      <c r="P193" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>85</v>
       </c>
@@ -10336,8 +11500,14 @@
       <c r="N194" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O194" t="s">
+        <v>461</v>
+      </c>
+      <c r="P194" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>255</v>
       </c>
@@ -10378,8 +11548,14 @@
       <c r="N195" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O195" t="s">
+        <v>461</v>
+      </c>
+      <c r="P195" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>118</v>
       </c>
@@ -10420,8 +11596,14 @@
       <c r="N196" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O196" t="s">
+        <v>461</v>
+      </c>
+      <c r="P196" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>198</v>
       </c>
@@ -10462,8 +11644,14 @@
       <c r="N197" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O197" t="s">
+        <v>461</v>
+      </c>
+      <c r="P197" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>89</v>
       </c>
@@ -10504,8 +11692,14 @@
       <c r="N198" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O198" t="s">
+        <v>461</v>
+      </c>
+      <c r="P198" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>110</v>
       </c>
@@ -10546,8 +11740,14 @@
       <c r="N199" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O199" t="s">
+        <v>461</v>
+      </c>
+      <c r="P199" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>451</v>
       </c>
@@ -10588,8 +11788,14 @@
       <c r="N200" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O200" t="s">
+        <v>461</v>
+      </c>
+      <c r="P200" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>199</v>
       </c>
@@ -10630,8 +11836,14 @@
       <c r="N201" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O201" t="s">
+        <v>453</v>
+      </c>
+      <c r="P201" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>169</v>
       </c>
@@ -10672,8 +11884,14 @@
       <c r="N202" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O202" t="s">
+        <v>453</v>
+      </c>
+      <c r="P202" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>0</v>
       </c>
@@ -10714,8 +11932,14 @@
       <c r="N203" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O203" t="s">
+        <v>461</v>
+      </c>
+      <c r="P203" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>132</v>
       </c>
@@ -10756,8 +11980,14 @@
       <c r="N204" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O204" t="s">
+        <v>461</v>
+      </c>
+      <c r="P204" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>58</v>
       </c>
@@ -10798,8 +12028,14 @@
       <c r="N205" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O205" t="s">
+        <v>461</v>
+      </c>
+      <c r="P205" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>310</v>
       </c>
@@ -10840,8 +12076,14 @@
       <c r="N206" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O206" t="s">
+        <v>461</v>
+      </c>
+      <c r="P206" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>162</v>
       </c>
@@ -10882,8 +12124,14 @@
       <c r="N207" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O207" t="s">
+        <v>453</v>
+      </c>
+      <c r="P207" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>108</v>
       </c>
@@ -10924,8 +12172,14 @@
       <c r="N208" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O208" t="s">
+        <v>461</v>
+      </c>
+      <c r="P208" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>407</v>
       </c>
@@ -10966,8 +12220,14 @@
       <c r="N209" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O209" t="s">
+        <v>461</v>
+      </c>
+      <c r="P209" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>146</v>
       </c>
@@ -11008,8 +12268,14 @@
       <c r="N210" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O210" t="s">
+        <v>461</v>
+      </c>
+      <c r="P210" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>339</v>
       </c>
@@ -11050,8 +12316,14 @@
       <c r="N211" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O211" t="s">
+        <v>461</v>
+      </c>
+      <c r="P211" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>51</v>
       </c>
@@ -11092,8 +12364,14 @@
       <c r="N212" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O212" t="s">
+        <v>453</v>
+      </c>
+      <c r="P212" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>186</v>
       </c>
@@ -11134,8 +12412,14 @@
       <c r="N213" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O213" t="s">
+        <v>461</v>
+      </c>
+      <c r="P213" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -11176,8 +12460,14 @@
       <c r="N214" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O214" t="s">
+        <v>461</v>
+      </c>
+      <c r="P214" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>403</v>
       </c>
@@ -11218,8 +12508,14 @@
       <c r="N215" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O215" t="s">
+        <v>461</v>
+      </c>
+      <c r="P215" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>148</v>
       </c>
@@ -11260,8 +12556,14 @@
       <c r="N216" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O216" t="s">
+        <v>461</v>
+      </c>
+      <c r="P216" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>431</v>
       </c>
@@ -11302,8 +12604,14 @@
       <c r="N217" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O217" t="s">
+        <v>461</v>
+      </c>
+      <c r="P217" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>105</v>
       </c>
@@ -11344,8 +12652,14 @@
       <c r="N218" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O218" t="s">
+        <v>461</v>
+      </c>
+      <c r="P218" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>445</v>
       </c>
@@ -11386,8 +12700,14 @@
       <c r="N219" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O219" t="s">
+        <v>461</v>
+      </c>
+      <c r="P219" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>30</v>
       </c>
@@ -11428,8 +12748,14 @@
       <c r="N220" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O220" t="s">
+        <v>461</v>
+      </c>
+      <c r="P220" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>379</v>
       </c>
@@ -11470,8 +12796,14 @@
       <c r="N221" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O221" t="s">
+        <v>461</v>
+      </c>
+      <c r="P221" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>28</v>
       </c>
@@ -11512,8 +12844,14 @@
       <c r="N222" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O222" t="s">
+        <v>461</v>
+      </c>
+      <c r="P222" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>188</v>
       </c>
@@ -11554,8 +12892,14 @@
       <c r="N223" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O223" t="s">
+        <v>461</v>
+      </c>
+      <c r="P223" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>201</v>
       </c>
@@ -11596,8 +12940,14 @@
       <c r="N224" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O224" t="s">
+        <v>461</v>
+      </c>
+      <c r="P224" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>150</v>
       </c>
@@ -11638,8 +12988,14 @@
       <c r="N225" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O225" t="s">
+        <v>461</v>
+      </c>
+      <c r="P225" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>375</v>
       </c>
@@ -11680,8 +13036,14 @@
       <c r="N226" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O226" t="s">
+        <v>461</v>
+      </c>
+      <c r="P226" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>385</v>
       </c>
@@ -11722,8 +13084,14 @@
       <c r="N227" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O227" t="s">
+        <v>461</v>
+      </c>
+      <c r="P227" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>381</v>
       </c>
@@ -11764,8 +13132,14 @@
       <c r="N228" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O228" t="s">
+        <v>461</v>
+      </c>
+      <c r="P228" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>377</v>
       </c>
@@ -11806,8 +13180,14 @@
       <c r="N229" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O229" t="s">
+        <v>461</v>
+      </c>
+      <c r="P229" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>399</v>
       </c>
@@ -11848,8 +13228,14 @@
       <c r="N230" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O230" t="s">
+        <v>461</v>
+      </c>
+      <c r="P230" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>264</v>
       </c>
@@ -11890,8 +13276,14 @@
       <c r="N231" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O231" t="s">
+        <v>461</v>
+      </c>
+      <c r="P231" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>39</v>
       </c>
@@ -11932,8 +13324,14 @@
       <c r="N232" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O232" t="s">
+        <v>461</v>
+      </c>
+      <c r="P232" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>325</v>
       </c>
@@ -11974,8 +13372,14 @@
       <c r="N233" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O233" t="s">
+        <v>461</v>
+      </c>
+      <c r="P233" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="234" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>348</v>
       </c>
@@ -12016,8 +13420,14 @@
       <c r="N234" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O234" t="s">
+        <v>461</v>
+      </c>
+      <c r="P234" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>300</v>
       </c>
@@ -12058,8 +13468,14 @@
       <c r="N235" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O235" t="s">
+        <v>461</v>
+      </c>
+      <c r="P235" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>298</v>
       </c>
@@ -12100,8 +13516,14 @@
       <c r="N236" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O236" t="s">
+        <v>461</v>
+      </c>
+      <c r="P236" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>284</v>
       </c>
@@ -12142,8 +13564,14 @@
       <c r="N237" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O237" t="s">
+        <v>461</v>
+      </c>
+      <c r="P237" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>278</v>
       </c>
@@ -12184,8 +13612,14 @@
       <c r="N238" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O238" t="s">
+        <v>461</v>
+      </c>
+      <c r="P238" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>280</v>
       </c>
@@ -12226,8 +13660,14 @@
       <c r="N239" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O239" t="s">
+        <v>461</v>
+      </c>
+      <c r="P239" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>286</v>
       </c>
@@ -12268,8 +13708,14 @@
       <c r="N240" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O240" t="s">
+        <v>461</v>
+      </c>
+      <c r="P240" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="241" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>288</v>
       </c>
@@ -12310,8 +13756,14 @@
       <c r="N241" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O241" t="s">
+        <v>461</v>
+      </c>
+      <c r="P241" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>290</v>
       </c>
@@ -12352,8 +13804,14 @@
       <c r="N242" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O242" t="s">
+        <v>461</v>
+      </c>
+      <c r="P242" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>296</v>
       </c>
@@ -12394,8 +13852,14 @@
       <c r="N243" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O243" t="s">
+        <v>461</v>
+      </c>
+      <c r="P243" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>367</v>
       </c>
@@ -12436,8 +13900,14 @@
       <c r="N244" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O244" t="s">
+        <v>461</v>
+      </c>
+      <c r="P244" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>365</v>
       </c>
@@ -12478,8 +13948,14 @@
       <c r="N245" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O245" t="s">
+        <v>461</v>
+      </c>
+      <c r="P245" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>304</v>
       </c>
@@ -12520,8 +13996,14 @@
       <c r="N246" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O246" t="s">
+        <v>461</v>
+      </c>
+      <c r="P246" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>245</v>
       </c>
@@ -12562,8 +14044,14 @@
       <c r="N247" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O247" t="s">
+        <v>461</v>
+      </c>
+      <c r="P247" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>350</v>
       </c>
@@ -12604,8 +14092,14 @@
       <c r="N248" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O248" t="s">
+        <v>461</v>
+      </c>
+      <c r="P248" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>433</v>
       </c>
@@ -12646,8 +14140,14 @@
       <c r="N249" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O249" t="s">
+        <v>461</v>
+      </c>
+      <c r="P249" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>362</v>
       </c>
@@ -12690,8 +14190,14 @@
       <c r="N250" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O250" t="s">
+        <v>461</v>
+      </c>
+      <c r="P250" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>122</v>
       </c>
@@ -12732,8 +14238,14 @@
       <c r="N251" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O251" t="s">
+        <v>461</v>
+      </c>
+      <c r="P251" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>276</v>
       </c>
@@ -12774,8 +14286,14 @@
       <c r="N252" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O252" t="s">
+        <v>461</v>
+      </c>
+      <c r="P252" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>78</v>
       </c>
@@ -12816,8 +14334,14 @@
       <c r="N253" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O253" t="s">
+        <v>461</v>
+      </c>
+      <c r="P253" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>93</v>
       </c>
@@ -12858,8 +14382,14 @@
       <c r="N254" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O254" t="s">
+        <v>461</v>
+      </c>
+      <c r="P254" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>508</v>
       </c>
@@ -12900,8 +14430,14 @@
       <c r="N255" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O255" t="s">
+        <v>461</v>
+      </c>
+      <c r="P255" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>509</v>
       </c>
@@ -12942,14 +14478,23 @@
       <c r="N256" t="s">
         <v>453</v>
       </c>
+      <c r="O256" t="s">
+        <v>461</v>
+      </c>
+      <c r="P256" t="s">
+        <v>461</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N256" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
-    <filterColumn colId="2">
+  <autoFilter ref="A1:P256" xr:uid="{045789F4-2A48-4566-BBEF-7A4CCFC6F4FC}">
+    <filterColumn colId="9">
       <filters>
-        <filter val="Iceland"/>
-        <filter val="Norway"/>
-        <filter val="Switzerland"/>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="14">
+      <filters>
+        <filter val="Y"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>